<commit_message>
battery scaling, update control mode functions
</commit_message>
<xml_diff>
--- a/node-firmware/tf-node-v0.1/TF Node v0.1 DEV Analog Data.xlsx
+++ b/node-firmware/tf-node-v0.1/TF Node v0.1 DEV Analog Data.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Dannemiller\Dropbox\Github\ThermoFlex\node-firmware\tf-node-v0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\priva\Dropbox\Github\ThermoFlex\node-firmware\tf-node-v0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B225AE-B2FD-4866-8B21-7AB0750B5AD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BE2084-7158-4CC1-9C59-51839D459993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2685" windowWidth="20970" windowHeight="15885" xr2:uid="{FFE93BE5-C805-44FA-B493-5CE708FF225C}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="9766" windowHeight="11363" xr2:uid="{FFE93BE5-C805-44FA-B493-5CE708FF225C}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery" sheetId="1" r:id="rId1"/>
     <sheet name="M1" sheetId="2" r:id="rId2"/>
+    <sheet name="M2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>Volts</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>Arduino Pin: A4</t>
+  </si>
+  <si>
+    <t>Arduino Pin: A3</t>
   </si>
 </sst>
 </file>
@@ -106,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -129,17 +133,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -338,43 +354,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>110</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>123</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>136</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>157</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>172</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>193</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>236</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>251</c:v>
+                  <c:v>133</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>269</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>345</c:v>
+                  <c:v>177</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>367</c:v>
+                  <c:v>211</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>403</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -386,43 +399,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>8.01</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.01</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.56</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.71</c:v>
+                  <c:v>2.93</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.25</c:v>
+                  <c:v>4.8899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.5</c:v>
+                  <c:v>7.11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.61</c:v>
+                  <c:v>9.5299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20</c:v>
+                  <c:v>11.01</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.67</c:v>
+                  <c:v>12.89</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.34</c:v>
+                  <c:v>15.42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.98</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>17.850000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -904,43 +914,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>119</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>132</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>145</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>166</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>182</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>202</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>246</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>261</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>280</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>355</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>377</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>400</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>413</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -952,43 +959,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>8.02</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.99</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.56</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.71</c:v>
+                  <c:v>2.93</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.24</c:v>
+                  <c:v>4.8899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.489999999999998</c:v>
+                  <c:v>7.11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.61</c:v>
+                  <c:v>9.5299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.010000000000002</c:v>
+                  <c:v>11.01</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.67</c:v>
+                  <c:v>12.89</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.33</c:v>
+                  <c:v>15.42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>28.98</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>30</c:v>
+                  <c:v>17.850000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -997,6 +1001,572 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-C4F3-4C11-8560-C6453503859B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1538044271"/>
+        <c:axId val="1538045231"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1538044271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1538045231"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1538045231"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Analog Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1538044271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>M2  Analog Read</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'M2'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.7291119860017496E-2"/>
+                  <c:y val="0.336777850685331"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="#,##0.00000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'M2'!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>238</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>266</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>351</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'M2'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1199999999999992</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.92</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>17.77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.86</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.78</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-058E-4D9B-AE53-6FD64A1231B2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1370,6 +1940,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -1909,6 +2519,544 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2552,6 +3700,49 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F0C720-1CE4-4E72-BEC9-AB0391951AFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>640555</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>30955</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FBAA7FB-BF0A-44C5-9E8F-E14E7ABEAC74}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2893,13 +4084,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1371DF55-078A-4A52-9D11-25721E637CC3}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2907,131 +4098,127 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2">
-        <v>8.01</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>123</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2">
-        <v>9.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
-        <v>136</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
-        <v>157</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2">
-        <v>11.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
-        <v>12.71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="B7" s="2">
-        <v>14.25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
-        <v>236</v>
+        <v>101</v>
       </c>
       <c r="B8" s="2">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
-        <v>251</v>
+        <v>133</v>
       </c>
       <c r="B9" s="2">
-        <v>18.61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.5299999999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
-        <v>269</v>
+        <v>152</v>
       </c>
       <c r="B10" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
-        <v>345</v>
+        <v>177</v>
       </c>
       <c r="B11" s="2">
-        <v>25.67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12.89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
-        <v>367</v>
+        <v>211</v>
       </c>
       <c r="B12" s="2">
-        <v>27.34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
-        <v>389</v>
+        <v>243</v>
       </c>
       <c r="B13" s="2">
-        <v>28.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>403</v>
-      </c>
-      <c r="B14" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17.850000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3047,15 +4234,234 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B626B3-E0A6-4F65-8779-F9F3B668751B}">
+  <dimension ref="A1:O21"/>
+  <sheetViews>
+    <sheetView zoomScale="81" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A2" s="2">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A3" s="2">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A4" s="2">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A5" s="2">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A6" s="2">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A7" s="2">
+        <v>80</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4.8899999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A8" s="2">
+        <v>109</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A9" s="2">
+        <v>141</v>
+      </c>
+      <c r="B9" s="2">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="N9" s="2">
+        <v>119</v>
+      </c>
+      <c r="O9" s="2">
+        <v>8.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A10" s="2">
+        <v>161</v>
+      </c>
+      <c r="B10" s="2">
+        <v>11.01</v>
+      </c>
+      <c r="N10" s="2">
+        <v>132</v>
+      </c>
+      <c r="O10" s="2">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A11" s="2">
+        <v>186</v>
+      </c>
+      <c r="B11" s="2">
+        <v>12.89</v>
+      </c>
+      <c r="N11" s="2">
+        <v>145</v>
+      </c>
+      <c r="O11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A12" s="2">
+        <v>220</v>
+      </c>
+      <c r="B12" s="2">
+        <v>15.42</v>
+      </c>
+      <c r="N12" s="2">
+        <v>166</v>
+      </c>
+      <c r="O12" s="2">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A13" s="2">
+        <v>252</v>
+      </c>
+      <c r="B13" s="2">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="N13" s="2">
+        <v>182</v>
+      </c>
+      <c r="O13" s="2">
+        <v>12.71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="N14" s="2">
+        <v>202</v>
+      </c>
+      <c r="O14" s="2">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N15" s="2">
+        <v>246</v>
+      </c>
+      <c r="O15" s="2">
+        <v>17.489999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N16" s="2">
+        <v>261</v>
+      </c>
+      <c r="O16" s="2">
+        <v>18.61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" s="2">
+        <v>280</v>
+      </c>
+      <c r="O17" s="2">
+        <v>20.010000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N18" s="2">
+        <v>355</v>
+      </c>
+      <c r="O18" s="2">
+        <v>25.67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N19" s="2">
+        <v>377</v>
+      </c>
+      <c r="O19" s="2">
+        <v>27.33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N20" s="2">
+        <v>400</v>
+      </c>
+      <c r="O20" s="2">
+        <v>28.98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="N21" s="2">
+        <v>413</v>
+      </c>
+      <c r="O21" s="2">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A719A87-ECBD-46A1-9B8E-AE4FD4EFCA78}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView zoomScale="81" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3063,113 +4469,113 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2">
-        <v>8.02</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
-        <v>145</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2">
-        <v>11.56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
-        <v>182</v>
+        <v>89</v>
       </c>
       <c r="B6" s="2">
-        <v>12.71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>202</v>
+        <v>124</v>
       </c>
       <c r="B7" s="2">
-        <v>14.24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9.1199999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
-        <v>246</v>
+        <v>148</v>
       </c>
       <c r="B8" s="2">
-        <v>17.489999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>261</v>
-      </c>
-      <c r="B9" s="2">
-        <v>18.61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>280</v>
-      </c>
-      <c r="B10" s="2">
-        <v>20.010000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10.92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="5">
+        <v>170</v>
+      </c>
+      <c r="B9" s="5">
+        <v>12.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="5">
+        <v>201</v>
+      </c>
+      <c r="B10" s="5">
+        <v>14.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
-        <v>355</v>
+        <v>238</v>
       </c>
       <c r="B11" s="2">
-        <v>25.67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17.77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
-        <v>377</v>
+        <v>266</v>
       </c>
       <c r="B12" s="2">
-        <v>27.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19.86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
-        <v>400</v>
+        <v>331</v>
       </c>
       <c r="B13" s="2">
-        <v>28.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24.78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
-        <v>413</v>
+        <v>351</v>
       </c>
       <c r="B14" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26.23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>